<commit_message>
fix bug and remove test data
</commit_message>
<xml_diff>
--- a/Data Files/Test Data_Partner_and_Player .xlsx
+++ b/Data Files/Test Data_Partner_and_Player .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.c/Katalon Studio/_Projects/Kataon_API_Testing/Data Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.c/git/Katalon_API_Testing/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3916EDB9-E276-6947-9496-75BB44717AE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8362E8C7-D8D6-7A40-B548-E2D35B58BA6A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4360" yWindow="-17540" windowWidth="28800" windowHeight="17540" xr2:uid="{A0C67E90-5654-D143-85D9-D30441451013}"/>
   </bookViews>
@@ -569,7 +569,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B3"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add test case for checking spin data by PTH, rgs-history
</commit_message>
<xml_diff>
--- a/Data Files/Test Data_Partner_and_Player .xlsx
+++ b/Data Files/Test Data_Partner_and_Player .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.c/git/Katalon_API_Testing/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8362E8C7-D8D6-7A40-B548-E2D35B58BA6A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D82FC36-5B2F-AD44-BF36-9101C8385D19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4360" yWindow="-17540" windowWidth="28800" windowHeight="17540" xr2:uid="{A0C67E90-5654-D143-85D9-D30441451013}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Partner Code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,10 @@
   </si>
   <si>
     <t>NG-1012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Katalon_Player_0001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -462,7 +466,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -504,7 +508,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -538,7 +542,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5">

</xml_diff>

<commit_message>
Support GT Wallet Separation
Add scripts for creating new player, wallet, increasing Gen-coin,
buying booster, checking game state, changing player status.
</commit_message>
<xml_diff>
--- a/Data Files/Test Data_Partner_and_Player .xlsx
+++ b/Data Files/Test Data_Partner_and_Player .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.c/git/Katalon_API_Testing/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D82FC36-5B2F-AD44-BF36-9101C8385D19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3D9C057-4F97-C64A-8229-CCA9E532D970}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4360" yWindow="-17540" windowWidth="28800" windowHeight="17540" xr2:uid="{A0C67E90-5654-D143-85D9-D30441451013}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Partner_Data" sheetId="1" r:id="rId1"/>
     <sheet name="Test_Account" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>